<commit_message>
make model with overfitting handling
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOKUMEN\Kuliah\Semester7\Pembelajaran Mesin\Prak. Pembelajaran Mesin\PraktikumML_073-076\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOKUMEN\Kuliah\Semester7\Pembelajaran Mesin\Prak. Pembelajaran Mesin\Tugas\PraktikumML_073-076\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D468545-8CD8-4A48-B08F-ACF4FFB86177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3567384-095B-4C58-B37A-F70B0994F5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1C0484A1-A412-45AA-BB4E-F656230E54A1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Task</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Modelling CNN</t>
   </si>
   <si>
-    <t>Frontend Web</t>
-  </si>
-  <si>
-    <t>Config Flask</t>
-  </si>
-  <si>
     <t>Aries</t>
   </si>
   <si>
@@ -63,10 +57,13 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Waiting</t>
-  </si>
-  <si>
     <t>On Going</t>
+  </si>
+  <si>
+    <t>Modelling CNN with overfiting handiling</t>
+  </si>
+  <si>
+    <t>Model Deploymet</t>
   </si>
 </sst>
 </file>
@@ -450,15 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A325FF50-11B5-488F-BAC0-85EF13CC405C}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
@@ -493,10 +490,10 @@
         <v>44492</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -510,45 +507,59 @@
         <v>44502</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>44528</v>
+        <v>44508</v>
       </c>
       <c r="C4" s="2">
-        <v>44536</v>
+        <v>44509</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>44537</v>
+        <v>44510</v>
       </c>
       <c r="C5" s="2">
-        <v>44543</v>
+        <v>44512</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
edit readme and sprint project
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOKUMEN\Kuliah\Semester7\Pembelajaran Mesin\Prak. Pembelajaran Mesin\Tugas\PraktikumML_073-076\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOKUMEN\Kuliah\Semester7\Pembelajaran Mesin\Prak. Pembelajaran Mesin\PraktikumML_073-076\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D56F428-3814-431E-93AD-0874ECCBE9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388AC19A-85CE-434F-83EB-EAF46FB90CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1C0484A1-A412-45AA-BB4E-F656230E54A1}"/>
   </bookViews>
@@ -66,7 +66,7 @@
     <t>Model Deploymet</t>
   </si>
   <si>
-    <t>Modelling Alexnet with Hyperparameter</t>
+    <t>Modelling Alexnet and Densenet201</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>